<commit_message>
FEAF: Correccion de objetos
Actualizacion de storeds para slots y agente default
</commit_message>
<xml_diff>
--- a/05 Manuales/Avances.xlsx
+++ b/05 Manuales/Avances.xlsx
@@ -995,7 +995,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D22" sqref="D22:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1004,7 @@
     <col min="2" max="2" width="57.42578125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="27" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>